<commit_message>
Free movement between 4 and 5
This solved the issue with overlapping stopovers. One more issue remaining where the model doesn't recognize shorter migrations; going to try converting dist_start to a regression cov
</commit_message>
<xml_diff>
--- a/5_state_transition_structure.xlsx
+++ b/5_state_transition_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umainesystem-my.sharepoint.com/personal/liam_berigan_maine_edu/Documents/MaineAnalysis/Projects/fac-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2559DAC5-8B22-4535-8DA2-2290A953E472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{2559DAC5-8B22-4535-8DA2-2290A953E472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22E69E18-90DC-4653-A2DE-200B36DDFD38}"/>
   <bookViews>
-    <workbookView xWindow="7428" yWindow="0" windowWidth="15708" windowHeight="12336" xr2:uid="{26575DA6-CB0D-4411-AB9B-D6587EA00E50}"/>
+    <workbookView minimized="1" xWindow="3492" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{26575DA6-CB0D-4411-AB9B-D6587EA00E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>pre</t>
   </si>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A421CBE-766F-4E23-8A7B-03F02A355FD1}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="M2" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,8 +652,8 @@
       <c r="S15">
         <v>-1000</v>
       </c>
-      <c r="T15">
-        <v>-1000</v>
+      <c r="T15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4-state model for spring females
4-state with almost all of the original variables. Is almost perfect, although I want to add residence time back in to see if it improves things further
</commit_message>
<xml_diff>
--- a/5_state_transition_structure.xlsx
+++ b/5_state_transition_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umainesystem-my.sharepoint.com/personal/liam_berigan_maine_edu/Documents/MaineAnalysis/Projects/fac-classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{2559DAC5-8B22-4535-8DA2-2290A953E472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22E69E18-90DC-4653-A2DE-200B36DDFD38}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{2559DAC5-8B22-4535-8DA2-2290A953E472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78729EFB-7B71-4C85-B083-1222F343C794}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3492" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{26575DA6-CB0D-4411-AB9B-D6587EA00E50}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15324" windowHeight="12336" xr2:uid="{26575DA6-CB0D-4411-AB9B-D6587EA00E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>pre</t>
   </si>
@@ -466,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A421CBE-766F-4E23-8A7B-03F02A355FD1}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,6 +656,106 @@
         <v>25</v>
       </c>
     </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" t="s">
+        <v>22</v>
+      </c>
+      <c r="S17" t="s">
+        <v>23</v>
+      </c>
+      <c r="T17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>-1000</v>
+      </c>
+      <c r="C18">
+        <v>-1000</v>
+      </c>
+      <c r="D18">
+        <v>-1000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>-1000</v>
+      </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18">
+        <v>-1000</v>
+      </c>
+      <c r="J18">
+        <v>-1000</v>
+      </c>
+      <c r="K18">
+        <v>-1000</v>
+      </c>
+      <c r="L18">
+        <v>-1000</v>
+      </c>
+      <c r="Q18">
+        <v>-1000</v>
+      </c>
+      <c r="R18">
+        <v>-1000</v>
+      </c>
+      <c r="S18">
+        <v>-1000</v>
+      </c>
+      <c r="T18" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>